<commit_message>
update stocks history, and add scalability
</commit_message>
<xml_diff>
--- a/graph.xlsx
+++ b/graph.xlsx
@@ -126,10 +126,10 @@
   <dimension ref="A1:D1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.27"/>

</xml_diff>